<commit_message>
added functionality for delete add
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -201,15 +201,18 @@
     <t>https://github.com/YanaSlavcheva/SoftUni-Work/tree/master/Angular-JS-Exam</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>I created half the project during the lab so half the project is committed at once
- - after the lab was finished</t>
+ - after the lab was finished, overall 4 days of work (except the lab)</t>
   </si>
   <si>
     <t>the project is commited on small portions
- - the way it was created by me</t>
-  </si>
-  <si>
-    <t>Yes</t>
+ - over 30 commits</t>
+  </si>
+  <si>
+    <t>Yes Half</t>
   </si>
 </sst>
 </file>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +770,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -778,7 +781,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -792,7 +795,7 @@
         <v>56</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -927,7 +930,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -937,7 +942,9 @@
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
@@ -969,7 +976,9 @@
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -979,7 +988,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -989,7 +1000,9 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1012,9 @@
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1056,9 @@
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1076,9 @@
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1110,7 +1129,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
@@ -1233,7 +1252,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
updated self evaluation protocol
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -208,11 +208,14 @@
  - over 30 commits</t>
   </si>
   <si>
-    <t>Yes Half</t>
-  </si>
-  <si>
     <t>I created half the project during the lab so half the project is committed at once
  - after the lab was finished, overall 4 days of work (+ 1 day from the lab)</t>
+  </si>
+  <si>
+    <t>paging-ът малко се счупи</t>
+  </si>
+  <si>
+    <t>дизайнът е responsive</t>
   </si>
 </sst>
 </file>
@@ -699,7 +702,7 @@
   <dimension ref="B2:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +784,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -816,7 +819,9 @@
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -1081,18 +1086,22 @@
         <v>27</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1102,7 +1111,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1123,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1122,7 +1135,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added creation of new category
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>дизайнът е responsive</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>Delete работи, но не се отваря delete screen</t>
   </si>
 </sst>
 </file>
@@ -701,15 +707,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1179,17 +1185,23 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1199,7 +1211,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added delete of category
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Delete работи (директно, без delete screen)</t>
+  </si>
+  <si>
+    <t>Започнато е</t>
   </si>
 </sst>
 </file>
@@ -707,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1172,9 @@
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
@@ -1227,13 +1232,17 @@
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added listing of towns
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -711,7 +711,7 @@
   <dimension ref="B2:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,13 +1246,17 @@
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added creation of towns
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -204,10 +204,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>the project is commited on small portions
- - over 30 commits</t>
-  </si>
-  <si>
     <t>I created half the project during the lab so half the project is committed at once
  - after the lab was finished, overall 4 days of work (+ 1 day from the lab)</t>
   </si>
@@ -225,6 +221,10 @@
   </si>
   <si>
     <t>Започнато е</t>
+  </si>
+  <si>
+    <t>the project is made and commited on small portions
+ - over 40 commits</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>56</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>28</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -1191,13 +1191,13 @@
         <v>36</v>
       </c>
       <c r="C42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>28</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -1241,13 +1241,13 @@
         <v>40</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added delete town functionality
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -711,7 +711,7 @@
   <dimension ref="B2:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1266,9 @@
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
updated the self evaluation card
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,11 +1288,15 @@
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="51" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">

</xml_diff>

<commit_message>
updated self evaluation card
</commit_message>
<xml_diff>
--- a/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
+++ b/Angular-JS-Exam/Self-Evaluation-Protocol/JS-SPA-Self-Evaluation-Protocol-Yana-Slavcheva.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -225,6 +225,12 @@
   <si>
     <t>the project is made and commited on small portions
  - over 40 commits</t>
+  </si>
+  <si>
+    <t>Website with uploaded project</t>
+  </si>
+  <si>
+    <t>http://store.slavcheva.net/#/</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -396,36 +402,45 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -700,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F51"/>
+  <dimension ref="B2:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,69 +751,65 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C8" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>50</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C9" s="6">
         <v>50</v>
@@ -806,47 +817,49 @@
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>50</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+    <row r="11" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
@@ -858,7 +871,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5">
         <v>5</v>
@@ -870,7 +883,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5">
         <v>5</v>
@@ -882,7 +895,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
         <v>5</v>
@@ -894,55 +907,55 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5">
         <v>10</v>
       </c>
-      <c r="C20" s="5">
-        <v>5</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5">
         <v>5</v>
@@ -954,7 +967,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5">
         <v>5</v>
@@ -966,7 +979,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="5">
         <v>5</v>
@@ -978,9 +991,11 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
@@ -988,11 +1003,9 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="5">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -1000,31 +1013,31 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="5">
         <v>5</v>
@@ -1036,7 +1049,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="5">
         <v>5</v>
@@ -1048,7 +1061,7 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" s="5">
         <v>5</v>
@@ -1060,7 +1073,7 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="5">
         <v>5</v>
@@ -1072,41 +1085,39 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5">
-        <v>5</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
+      <c r="C33" s="5">
+        <v>5</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B34" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>60</v>
@@ -1114,11 +1125,13 @@
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="7"/>
+      <c r="E35" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>60</v>
@@ -1130,7 +1143,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>60</v>
@@ -1142,7 +1155,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>60</v>
@@ -1154,7 +1167,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>60</v>
@@ -1166,55 +1179,55 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>64</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>60</v>
@@ -1226,45 +1239,45 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>64</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C46" s="7"/>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>60</v>
@@ -1276,9 +1289,11 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
@@ -1286,45 +1301,57 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="7" t="s">
+      <c r="D51" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
+    <row r="52" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="11">
-        <f>SUM(C6:C50)</f>
+      <c r="C52" s="11">
+        <f>SUM(C6:C51)</f>
         <v>225</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D52" s="11">
         <v>430</v>
       </c>
-      <c r="E51" s="1"/>
+      <c r="E52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B33:E33"/>
+  <mergeCells count="8">
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2" location="/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>